<commit_message>
sehr gute version. fragen inkl korrekter antwort und result screen. next-step: syncfusion
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\AndroidStudioProjects\advanced_quiz_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81275243-4A99-462A-9440-5BA8A653D8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24629C46-10F0-4BDA-A33B-63FE33B963E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3375" yWindow="30" windowWidth="21600" windowHeight="11385" xr2:uid="{C43A4763-3D82-49CC-8768-BEB4E5CE4DF9}"/>
   </bookViews>
@@ -35,66 +35,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Lieblingsfarbe</t>
+    <t>2 + 2 =</t>
   </si>
   <si>
-    <t>rot</t>
+    <t>2 * 2 =</t>
   </si>
   <si>
-    <t>gruen</t>
+    <t>2 - 2 =</t>
   </si>
   <si>
-    <t>blau</t>
-  </si>
-  <si>
-    <t>gelb</t>
-  </si>
-  <si>
-    <t>Lieblingstier</t>
-  </si>
-  <si>
-    <t>Stier</t>
-  </si>
-  <si>
-    <t>Hase</t>
-  </si>
-  <si>
-    <t>Ente</t>
-  </si>
-  <si>
-    <t>Gazelle</t>
-  </si>
-  <si>
-    <t>Lieblingsessen</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Burger</t>
-  </si>
-  <si>
-    <t>Pasta</t>
-  </si>
-  <si>
-    <t>Kuchen</t>
-  </si>
-  <si>
-    <t>Mojito</t>
-  </si>
-  <si>
-    <t>Pina Colada</t>
-  </si>
-  <si>
-    <t>Bier</t>
-  </si>
-  <si>
-    <t>Wein</t>
-  </si>
-  <si>
-    <t>Lieblingsgetränk</t>
+    <t xml:space="preserve">4 - 3 = </t>
   </si>
 </sst>
 </file>
@@ -136,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -452,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F8AFC0-CD39-48C0-8A6F-14E5DC30DBF4}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,72 +419,84 @@
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>6</v>
+      </c>
+      <c r="D1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1">
+        <v>-4</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>-8</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>